<commit_message>
p7 Final project fourth upload
</commit_message>
<xml_diff>
--- a/p7/Final+Project+Baseline+Values.xlsx
+++ b/p7/Final+Project+Baseline+Values.xlsx
@@ -100,7 +100,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -108,7 +108,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,8 +136,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,33 +190,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -198,53 +215,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,31 +259,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,43 +385,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -344,102 +440,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,60 +450,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -526,7 +472,37 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,6 +521,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -556,10 +556,10 @@
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -568,7 +568,7 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -577,124 +577,124 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1016,13 +1016,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="55.5714285714286" customWidth="1"/>
   </cols>
@@ -1157,10 +1157,10 @@
         <v>0.0202</v>
       </c>
       <c r="C17">
-        <v>4737818</v>
-      </c>
-    </row>
-    <row r="18" customHeight="1" spans="1:3">
+        <v>645875</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:4">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1170,6 +1170,9 @@
       </c>
       <c r="C18">
         <v>4741212</v>
+      </c>
+      <c r="D18">
+        <v>39115</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:3">

</xml_diff>